<commit_message>
finally got the right size
</commit_message>
<xml_diff>
--- a/accuracies-new-poster.xlsx
+++ b/accuracies-new-poster.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simbe\Desktop\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBC0D6A8-DE0D-46A1-BC3B-789F7D6039CA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A74BF31F-A7EE-4E30-A84D-EB8A0DEEAE00}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -219,7 +219,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="46">
+  <borders count="43">
     <border>
       <left/>
       <right/>
@@ -238,15 +238,6 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right/>
       <top/>
       <bottom style="medium">
@@ -364,17 +355,6 @@
       <top style="dashed">
         <color theme="0" tint="-0.499984740745262"/>
       </top>
-      <bottom style="dashed">
-        <color theme="0" tint="-0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
       <bottom style="dashed">
         <color theme="0" tint="-0.499984740745262"/>
       </bottom>
@@ -647,17 +627,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -776,102 +745,105 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="7" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="8" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="8" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -880,110 +852,98 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="8" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="117"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="117"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="9" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="117"/>
-    </xf>
-    <xf numFmtId="2" fontId="9" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="117"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1325,8 +1285,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13:I14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1343,17 +1303,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="51"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="60"/>
       <c r="J1" s="13"/>
       <c r="K1" s="13"/>
       <c r="L1" s="13"/>
@@ -1374,21 +1334,21 @@
       <c r="AB1" s="13"/>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="44"/>
-      <c r="C2" s="52" t="s">
+      <c r="B2" s="53"/>
+      <c r="C2" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="63"/>
-      <c r="E2" s="60"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="64"/>
       <c r="F2" s="16"/>
-      <c r="G2" s="52" t="s">
+      <c r="G2" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="63"/>
-      <c r="I2" s="60"/>
+      <c r="H2" s="66"/>
+      <c r="I2" s="64"/>
       <c r="J2" s="13"/>
       <c r="K2" s="13"/>
       <c r="L2" s="13"/>
@@ -1409,23 +1369,23 @@
       <c r="AB2" s="13"/>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A3" s="45"/>
-      <c r="B3" s="46"/>
-      <c r="C3" s="58" t="s">
+      <c r="A3" s="54"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="62" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="67" t="s">
+      <c r="D3" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="61"/>
+      <c r="E3" s="49"/>
       <c r="F3" s="18"/>
-      <c r="G3" s="58" t="s">
+      <c r="G3" s="62" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="67" t="s">
+      <c r="H3" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="61"/>
+      <c r="I3" s="49"/>
       <c r="J3" s="13"/>
       <c r="K3" s="13"/>
       <c r="L3" s="13"/>
@@ -1446,9 +1406,9 @@
       <c r="AB3" s="13"/>
     </row>
     <row r="4" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="47"/>
-      <c r="B4" s="48"/>
-      <c r="C4" s="59"/>
+      <c r="A4" s="56"/>
+      <c r="B4" s="57"/>
+      <c r="C4" s="63"/>
       <c r="D4" s="17" t="s">
         <v>13</v>
       </c>
@@ -1456,7 +1416,7 @@
         <v>10</v>
       </c>
       <c r="F4" s="29"/>
-      <c r="G4" s="59"/>
+      <c r="G4" s="63"/>
       <c r="H4" s="17" t="s">
         <v>13</v>
       </c>
@@ -1483,13 +1443,13 @@
       <c r="AB4" s="13"/>
     </row>
     <row r="5" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="52" t="s">
+      <c r="A5" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="60" t="s">
+      <c r="B5" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="55">
+      <c r="C5" s="45">
         <v>1.49</v>
       </c>
       <c r="D5" s="33" t="s">
@@ -1499,7 +1459,7 @@
         <v>100</v>
       </c>
       <c r="F5" s="30"/>
-      <c r="G5" s="55">
+      <c r="G5" s="45">
         <v>8.3000000000000007</v>
       </c>
       <c r="H5" s="33" t="s">
@@ -1528,9 +1488,9 @@
       <c r="AB5" s="13"/>
     </row>
     <row r="6" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="53"/>
-      <c r="B6" s="61"/>
-      <c r="C6" s="56"/>
+      <c r="A6" s="61"/>
+      <c r="B6" s="49"/>
+      <c r="C6" s="46"/>
       <c r="D6" s="34" t="s">
         <v>5</v>
       </c>
@@ -1538,7 +1498,7 @@
         <v>100</v>
       </c>
       <c r="F6" s="31"/>
-      <c r="G6" s="56"/>
+      <c r="G6" s="46"/>
       <c r="H6" s="34" t="s">
         <v>5</v>
       </c>
@@ -1565,9 +1525,9 @@
       <c r="AB6" s="13"/>
     </row>
     <row r="7" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="53"/>
-      <c r="B7" s="62"/>
-      <c r="C7" s="57"/>
+      <c r="A7" s="61"/>
+      <c r="B7" s="65"/>
+      <c r="C7" s="47"/>
       <c r="D7" s="35" t="s">
         <v>6</v>
       </c>
@@ -1575,7 +1535,7 @@
         <v>100</v>
       </c>
       <c r="F7" s="32"/>
-      <c r="G7" s="57"/>
+      <c r="G7" s="47"/>
       <c r="H7" s="35" t="s">
         <v>6</v>
       </c>
@@ -1602,7 +1562,7 @@
       <c r="AB7" s="13"/>
     </row>
     <row r="8" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="54"/>
+      <c r="A8" s="44"/>
       <c r="B8" s="7" t="s">
         <v>12</v>
       </c>
@@ -1645,13 +1605,13 @@
       <c r="AB8" s="13"/>
     </row>
     <row r="9" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="52" t="s">
+      <c r="A9" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="60" t="s">
+      <c r="B9" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="55">
+      <c r="C9" s="45">
         <v>3.7</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -1661,7 +1621,7 @@
         <v>4.5</v>
       </c>
       <c r="F9" s="37"/>
-      <c r="G9" s="64">
+      <c r="G9" s="45">
         <v>12.3</v>
       </c>
       <c r="H9" s="1" t="s">
@@ -1690,9 +1650,9 @@
       <c r="AB9" s="13"/>
     </row>
     <row r="10" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="53"/>
-      <c r="B10" s="61"/>
-      <c r="C10" s="56"/>
+      <c r="A10" s="61"/>
+      <c r="B10" s="49"/>
+      <c r="C10" s="46"/>
       <c r="D10" s="4" t="s">
         <v>5</v>
       </c>
@@ -1700,7 +1660,7 @@
         <v>7.3</v>
       </c>
       <c r="F10" s="38"/>
-      <c r="G10" s="65"/>
+      <c r="G10" s="46"/>
       <c r="H10" s="4" t="s">
         <v>5</v>
       </c>
@@ -1727,9 +1687,9 @@
       <c r="AB10" s="13"/>
     </row>
     <row r="11" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="53"/>
-      <c r="B11" s="62"/>
-      <c r="C11" s="57"/>
+      <c r="A11" s="61"/>
+      <c r="B11" s="65"/>
+      <c r="C11" s="47"/>
       <c r="D11" s="2" t="s">
         <v>6</v>
       </c>
@@ -1737,7 +1697,7 @@
         <v>5.4</v>
       </c>
       <c r="F11" s="39"/>
-      <c r="G11" s="66"/>
+      <c r="G11" s="47"/>
       <c r="H11" s="2" t="s">
         <v>6</v>
       </c>
@@ -1764,7 +1724,7 @@
       <c r="AB11" s="13"/>
     </row>
     <row r="12" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="54"/>
+      <c r="A12" s="44"/>
       <c r="B12" s="9" t="s">
         <v>12</v>
       </c>
@@ -1807,7 +1767,7 @@
       <c r="AB12" s="13"/>
     </row>
     <row r="13" spans="1:28" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="52" t="s">
+      <c r="A13" s="43" t="s">
         <v>17</v>
       </c>
       <c r="B13" s="19" t="s">
@@ -1819,7 +1779,7 @@
       <c r="D13" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="E13" s="68"/>
+      <c r="E13" s="50"/>
       <c r="F13" s="41"/>
       <c r="G13" s="20">
         <v>54.6</v>
@@ -1827,7 +1787,7 @@
       <c r="H13" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="I13" s="68"/>
+      <c r="I13" s="50"/>
       <c r="J13" s="13"/>
       <c r="K13" s="13"/>
       <c r="L13" s="13"/>
@@ -1848,7 +1808,7 @@
       <c r="AB13" s="13"/>
     </row>
     <row r="14" spans="1:28" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="54"/>
+      <c r="A14" s="44"/>
       <c r="B14" s="9" t="s">
         <v>12</v>
       </c>
@@ -1858,7 +1818,7 @@
       <c r="D14" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E14" s="69"/>
+      <c r="E14" s="51"/>
       <c r="F14" s="42"/>
       <c r="G14" s="21">
         <v>55.3</v>
@@ -1866,7 +1826,7 @@
       <c r="H14" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="I14" s="69"/>
+      <c r="I14" s="51"/>
       <c r="J14" s="13"/>
       <c r="K14" s="13"/>
       <c r="L14" s="13"/>
@@ -1887,7 +1847,7 @@
       <c r="AB14" s="13"/>
     </row>
     <row r="15" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="52" t="s">
+      <c r="A15" s="43" t="s">
         <v>18</v>
       </c>
       <c r="B15" s="19" t="s">
@@ -1899,7 +1859,7 @@
       <c r="D15" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="E15" s="68" t="s">
+      <c r="E15" s="50" t="s">
         <v>19</v>
       </c>
       <c r="F15" s="41"/>
@@ -1909,7 +1869,7 @@
       <c r="H15" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="I15" s="68" t="s">
+      <c r="I15" s="50" t="s">
         <v>19</v>
       </c>
       <c r="J15" s="13"/>
@@ -1932,7 +1892,7 @@
       <c r="AB15" s="13"/>
     </row>
     <row r="16" spans="1:28" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="54"/>
+      <c r="A16" s="44"/>
       <c r="B16" s="9" t="s">
         <v>12</v>
       </c>
@@ -1942,7 +1902,7 @@
       <c r="D16" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E16" s="69"/>
+      <c r="E16" s="51"/>
       <c r="F16" s="42"/>
       <c r="G16" s="21">
         <v>90.3</v>
@@ -1950,7 +1910,7 @@
       <c r="H16" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="I16" s="69"/>
+      <c r="I16" s="51"/>
       <c r="J16" s="13"/>
       <c r="K16" s="13"/>
       <c r="L16" s="13"/>
@@ -1971,7 +1931,7 @@
       <c r="AB16" s="13"/>
     </row>
     <row r="17" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="52" t="s">
+      <c r="A17" s="43" t="s">
         <v>9</v>
       </c>
       <c r="B17" s="8" t="s">
@@ -2016,7 +1976,7 @@
       <c r="AB17" s="13"/>
     </row>
     <row r="18" spans="1:28" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="54"/>
+      <c r="A18" s="44"/>
       <c r="B18" s="9" t="s">
         <v>12</v>
       </c>
@@ -2060,6 +2020,13 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="G3:G4"/>
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="G5:G7"/>
     <mergeCell ref="D3:E3"/>
@@ -2071,18 +2038,11 @@
     <mergeCell ref="I13:I14"/>
     <mergeCell ref="E13:E14"/>
     <mergeCell ref="A2:B4"/>
-    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="G9:G11"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="B9:B11"/>
     <mergeCell ref="A9:A12"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="A5:A8"/>
     <mergeCell ref="C5:C7"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="G9:G11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>